<commit_message>
Motor works good at 100 ms
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Продумываю общую структуру, выбираю компоненты</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Физический движок</t>
+  </si>
+  <si>
+    <t>Поставил двигатель</t>
+  </si>
+  <si>
+    <t>Тестирование двигателя</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +486,29 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="A6" s="2">
+        <v>42813</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42815</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>